<commit_message>
adds additional year of riverside data
</commit_message>
<xml_diff>
--- a/data/homelessness/school-homelessness/files_as_provided/RiversideUSD.xlsx
+++ b/data/homelessness/school-homelessness/files_as_provided/RiversideUSD.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Records Requests\PRA Requests\Mendelson KPCC June 2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DFS-67-SERVER02\59Share\Homeless-AB 490 Files and Forms\Homeless Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Annual Comparison" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="79">
   <si>
     <t>Grade Level</t>
   </si>
@@ -260,6 +260,15 @@
   </si>
   <si>
     <t>C) Number of Homeless children/youth that met or exceeded State proficiency</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>Preschool</t>
+  </si>
+  <si>
+    <t>Pending information</t>
   </si>
 </sst>
 </file>
@@ -283,12 +292,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -303,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -330,11 +345,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
+  <dxfs count="49">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -716,6 +737,66 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -729,18 +810,2700 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Number of Homeless Youth</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Served by Grade</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Under Age 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Preschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TK</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kindergarten</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>257</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>212</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>205</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>185</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>157</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>163</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>167</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>131</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>135</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ungraded</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent5">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="80000"/>
+                <a:lumOff val="20000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Youth Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2415</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="123942304"/>
+        <c:axId val="123942696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="123942304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="123942696"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="123942696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="123942304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Homeless Students Served by Residency</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Type</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2015-2016'!$B$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of Homeless Students Served</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'2015-2016'!$A$29:$A$33</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Shelters (100)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Doubled-Up (120)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Unsheltered (130)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Hotels/Motels (110)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2015-2016'!$B$29:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2213</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2415</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A29:B34" totalsRowShown="0" headerRowDxfId="42">
-  <autoFilter ref="A29:B34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A28:B33" totalsRowShown="0" headerRowDxfId="48">
+  <autoFilter ref="A28:B33"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Type of Residency"/>
-    <tableColumn id="2" name="Number of Homeless Students Served" dataDxfId="41"/>
+    <tableColumn id="2" name="Number of Homeless Students Served" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table16" displayName="Table16" ref="A47:B53" totalsRowShown="0">
+  <autoFilter ref="A47:B53"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Barriers"/>
+    <tableColumn id="2" name="Applicable"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table212" displayName="Table212" ref="A1:B18" totalsRowShown="0" headerRowDxfId="31">
+  <autoFilter ref="A1:B18"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Grade Level"/>
+    <tableColumn id="2" name="Number of Homeless Youth Served" dataDxfId="30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table313" displayName="Table313" ref="A20:B25" totalsRowShown="0" headerRowDxfId="29">
+  <autoFilter ref="A20:B25"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Subpopulations"/>
+    <tableColumn id="2" name="Number of Homeless Students Served" dataDxfId="28"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16" name="Table117" displayName="Table117" ref="A29:B34" totalsRowShown="0" headerRowDxfId="27">
   <autoFilter ref="A29:B34"/>
   <tableColumns count="2">
@@ -751,7 +3514,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Table218" displayName="Table218" ref="A1:B18" totalsRowShown="0" headerRowDxfId="25">
   <autoFilter ref="A1:B18"/>
   <tableColumns count="2">
@@ -762,7 +3525,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="18" name="Table319" displayName="Table319" ref="A20:B25" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A20:B25"/>
   <tableColumns count="2">
@@ -773,7 +3536,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="19" name="Table120" displayName="Table120" ref="A20:B25" totalsRowShown="0" headerRowDxfId="21">
   <autoFilter ref="A20:B25"/>
   <tableColumns count="2">
@@ -784,7 +3547,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Table221" displayName="Table221" ref="A1:B18" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="A1:B18"/>
   <tableColumns count="2">
@@ -795,7 +3558,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22" name="Table1523" displayName="Table1523" ref="A20:B25" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A20:B25"/>
   <tableColumns count="2">
@@ -806,7 +3569,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23" name="Table2624" displayName="Table2624" ref="A1:B18" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:B18"/>
   <tableColumns count="2">
@@ -817,7 +3580,18 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:B19" totalsRowShown="0" headerRowDxfId="46">
+  <autoFilter ref="A1:B19"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Grade Level"/>
+    <tableColumn id="2" name="Number of Homeless Youth Served" dataDxfId="45"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table1515" displayName="Table1515" ref="A10:B15" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A10:B15"/>
   <tableColumns count="2">
@@ -828,7 +3602,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="21" name="Table2622" displayName="Table2622" ref="A1:B8" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:B8"/>
   <tableColumns count="2">
@@ -839,7 +3613,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25" name="Table25" displayName="Table25" ref="A17:B19" totalsRowShown="0">
   <autoFilter ref="A17:B19"/>
   <tableColumns count="2">
@@ -850,18 +3624,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A1:B18" totalsRowShown="0" headerRowDxfId="40">
-  <autoFilter ref="A1:B18"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Grade Level"/>
-    <tableColumn id="2" name="Number of Homeless Youth Served" dataDxfId="39"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26" name="Table27" displayName="Table27" ref="A21:B25" totalsRowShown="0">
   <autoFilter ref="A21:B25"/>
   <tableColumns count="2">
@@ -872,7 +3635,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="27" name="Table1328" displayName="Table1328" ref="A27:B45" totalsRowShown="0" headerRowDxfId="7">
   <autoFilter ref="A27:B45"/>
   <tableColumns count="2">
@@ -883,7 +3646,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="28" name="Table1629" displayName="Table1629" ref="A47:B53" totalsRowShown="0">
   <autoFilter ref="A47:B53"/>
   <tableColumns count="2">
@@ -894,7 +3657,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="29" name="Table30" displayName="Table30" ref="A56:D67" totalsRowShown="0" dataDxfId="3">
   <autoFilter ref="A56:D67"/>
   <tableColumns count="4">
@@ -908,6 +3671,39 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A21:B26" totalsRowShown="0" headerRowDxfId="44">
+  <autoFilter ref="A21:B26"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Subpopulations"/>
+    <tableColumn id="2" name="Number of Homeless Students Served" dataDxfId="43"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table15" displayName="Table15" ref="A29:B34" totalsRowShown="0" headerRowDxfId="42">
+  <autoFilter ref="A29:B34"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Type of Residency"/>
+    <tableColumn id="2" name="Number of Homeless Students Served" dataDxfId="41"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table26" displayName="Table26" ref="A1:B18" totalsRowShown="0" headerRowDxfId="40">
+  <autoFilter ref="A1:B18"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Grade Level"/>
+    <tableColumn id="2" name="Number of Homeless Youth Served" dataDxfId="39"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table37" displayName="Table37" ref="A20:B25" totalsRowShown="0" headerRowDxfId="38">
   <autoFilter ref="A20:B25"/>
   <tableColumns count="2">
@@ -918,7 +3714,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table29" displayName="Table29" ref="A1:B18" totalsRowShown="0" headerRowDxfId="36">
   <autoFilter ref="A1:B18"/>
   <tableColumns count="2">
@@ -929,7 +3725,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table310" displayName="Table310" ref="A20:B25" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A20:B25"/>
   <tableColumns count="2">
@@ -940,45 +3736,12 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="A27:B45" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="A27:B45"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Services and Activities Provided by McKinney-Vento"/>
     <tableColumn id="2" name="Applicable"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table16" displayName="Table16" ref="A47:B53" totalsRowShown="0">
-  <autoFilter ref="A47:B53"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Barriers"/>
-    <tableColumn id="2" name="Applicable"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table212" displayName="Table212" ref="A1:B18" totalsRowShown="0" headerRowDxfId="31">
-  <autoFilter ref="A1:B18"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Grade Level"/>
-    <tableColumn id="2" name="Number of Homeless Youth Served" dataDxfId="30"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table313" displayName="Table313" ref="A20:B25" totalsRowShown="0" headerRowDxfId="29">
-  <autoFilter ref="A20:B25"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Subpopulations"/>
-    <tableColumn id="2" name="Number of Homeless Students Served" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1261,14 +4024,266 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>6</v>
+      </c>
+      <c r="B11" s="2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>7</v>
+      </c>
+      <c r="B12" s="2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>10</v>
+      </c>
+      <c r="B15" s="2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2">
+        <f>SUBTOTAL(109,B2:B18)</f>
+        <v>2415</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="2">
+        <f>SUBTOTAL(109,B29:B32)</f>
+        <v>2415</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="1" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
   <headerFooter>
@@ -1277,6 +4292,12 @@
 CDE Annual Homeless Education Data Collection</oddHeader>
     <oddFooter>&amp;L&amp;9&amp;Z&amp;F</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
+  <tableParts count="3">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1284,8 +4305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,24 +4480,16 @@
       <c r="A22" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>71</v>
-      </c>
+      <c r="B23" s="10"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1558,8 +4571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:XFD27"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2478,7 +5491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -2702,7 +5715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -2925,7 +5938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>

</xml_diff>